<commit_message>
new hybrid model (test with mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-5.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-5.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="mae" sheetId="1" r:id="rId1"/>
+    <sheet name="mae and mse" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Random Forest-100 (superdataset-21.csv without cons)</t>
   </si>
@@ -53,11 +53,20 @@
   <si>
     <t>Class F1</t>
   </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -115,6 +124,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -160,7 +175,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>mae!$H$63</c:f>
+              <c:f>'mae and mse'!$H$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -251,7 +266,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>mae!$I$62:$J$62</c:f>
+              <c:f>'mae and mse'!$I$62:$J$62</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -265,7 +280,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mae!$I$63:$J$63</c:f>
+              <c:f>'mae and mse'!$I$63:$J$63</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
@@ -289,7 +304,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>mae!$H$64</c:f>
+              <c:f>'mae and mse'!$H$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,7 +395,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>mae!$I$62:$J$62</c:f>
+              <c:f>'mae and mse'!$I$62:$J$62</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -394,7 +409,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mae!$I$64:$J$64</c:f>
+              <c:f>'mae and mse'!$I$64:$J$64</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1427,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:M65"/>
+  <dimension ref="D4:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,9 +1454,13 @@
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1450,8 +1469,16 @@
         <v>5</v>
       </c>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="T4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -1469,8 +1496,22 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>1</v>
       </c>
@@ -1489,15 +1530,30 @@
       <c r="K6" s="3">
         <v>115.8061468994582</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M6" s="4">
-        <f>L6*100</f>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="4"/>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>8.3755556994745669E-5</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>7.7074917629469655E-4</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1</v>
+      </c>
+      <c r="U6" s="6">
+        <v>1.2446644894602849E-4</v>
+      </c>
+      <c r="V6" s="6">
+        <v>6.1796445250980961E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f>D6+1</f>
         <v>2</v>
@@ -1518,17 +1574,34 @@
       <c r="K7" s="3">
         <v>116.9780433473811</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M7" s="4">
-        <f t="shared" ref="M7:M55" si="0">L7*100</f>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="4"/>
+      <c r="O7" s="2">
+        <f>O6+1</f>
+        <v>2</v>
+      </c>
+      <c r="P7" s="6">
+        <v>9.0436859233494128E-5</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>7.1527881066906353E-4</v>
+      </c>
+      <c r="T7" s="2">
+        <f>T6+1</f>
+        <v>2</v>
+      </c>
+      <c r="U7" s="6">
+        <v>1.1684232182386179E-4</v>
+      </c>
+      <c r="V7" s="6">
+        <v>9.0555319806772424E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
-        <f t="shared" ref="D8:D55" si="1">D7+1</f>
+        <f t="shared" ref="D8:D55" si="0">D7+1</f>
         <v>3</v>
       </c>
       <c r="E8" s="3">
@@ -1538,7 +1611,7 @@
         <v>143.13598028477551</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8:I55" si="2">I7+1</f>
+        <f t="shared" ref="I8:I55" si="1">I7+1</f>
         <v>3</v>
       </c>
       <c r="J8" s="3">
@@ -1547,17 +1620,34 @@
       <c r="K8" s="3">
         <v>118.7151414810355</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="5">
         <v>0.99439775910364148</v>
       </c>
-      <c r="M8" s="4">
-        <f t="shared" si="0"/>
-        <v>99.439775910364148</v>
-      </c>
-    </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="4"/>
+      <c r="O8" s="2">
+        <f t="shared" ref="O8:O55" si="2">O7+1</f>
+        <v>3</v>
+      </c>
+      <c r="P8" s="6">
+        <v>8.5378916092632547E-5</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>5.7510483607643812E-4</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" ref="T8:T55" si="3">T7+1</f>
+        <v>3</v>
+      </c>
+      <c r="U8" s="6">
+        <v>1.3064811918610399E-4</v>
+      </c>
+      <c r="V8" s="6">
+        <v>6.1581285621312588E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E9" s="3">
@@ -1567,7 +1657,7 @@
         <v>147.5578587075575</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J9" s="3">
@@ -1576,17 +1666,34 @@
       <c r="K9" s="3">
         <v>116.12380493678511</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="5">
         <v>0.99581589958158989</v>
       </c>
-      <c r="M9" s="4">
-        <f t="shared" si="0"/>
-        <v>99.581589958158986</v>
-      </c>
-    </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="4"/>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P9" s="6">
+        <v>8.996768063780694E-5</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>4.450114444867556E-4</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U9" s="6">
+        <v>1.2907266383490931E-4</v>
+      </c>
+      <c r="V9" s="6">
+        <v>8.2228677010219174E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E10" s="3">
@@ -1596,7 +1703,7 @@
         <v>150.0395071193866</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J10" s="3">
@@ -1605,17 +1712,34 @@
       <c r="K10" s="3">
         <v>106.94900060204699</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M10" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="4"/>
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="6">
+        <v>8.8182460020571485E-5</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>4.8602174961767349E-4</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U10" s="6">
+        <v>1.196053616554614E-4</v>
+      </c>
+      <c r="V10" s="6">
+        <v>1.131388841680097E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E11" s="3">
@@ -1625,7 +1749,7 @@
         <v>151.0301150054764</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J11" s="3">
@@ -1634,17 +1758,34 @@
       <c r="K11" s="3">
         <v>118.33442504515349</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="5">
         <v>0.99580419580419577</v>
       </c>
-      <c r="M11" s="4">
-        <f t="shared" si="0"/>
-        <v>99.580419580419573</v>
-      </c>
-    </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="4"/>
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P11" s="6">
+        <v>8.9265470268447413E-5</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>6.2101818325250549E-4</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U11" s="6">
+        <v>1.150768396915385E-4</v>
+      </c>
+      <c r="V11" s="6">
+        <v>8.7877762403024379E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E12" s="3">
@@ -1654,7 +1795,7 @@
         <v>144.29275465498361</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J12" s="3">
@@ -1663,17 +1804,34 @@
       <c r="K12" s="3">
         <v>113.3242323901264</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="5">
         <v>0.99300699300699313</v>
       </c>
-      <c r="M12" s="4">
-        <f t="shared" si="0"/>
-        <v>99.300699300699307</v>
-      </c>
-    </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="4"/>
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="P12" s="6">
+        <v>9.7277323009712033E-5</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>4.5673758593831423E-4</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U12" s="6">
+        <v>1.3179345133859961E-4</v>
+      </c>
+      <c r="V12" s="6">
+        <v>8.1214201809106225E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E13" s="3">
@@ -1683,7 +1841,7 @@
         <v>144.4272289156626</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J13" s="3">
@@ -1692,17 +1850,34 @@
       <c r="K13" s="3">
         <v>114.8426128838049</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="5">
         <v>0.99580419580419577</v>
       </c>
-      <c r="M13" s="4">
-        <f t="shared" si="0"/>
-        <v>99.580419580419573</v>
-      </c>
-    </row>
-    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P13" s="6">
+        <v>8.9035898344543845E-5</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>4.9345746450208555E-4</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U13" s="6">
+        <v>1.27837345502081E-4</v>
+      </c>
+      <c r="V13" s="6">
+        <v>6.5823873704807818E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E14" s="3">
@@ -1712,7 +1887,7 @@
         <v>148.92030668127049</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J14" s="3">
@@ -1721,17 +1896,34 @@
       <c r="K14" s="3">
         <v>114.4051053582179</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M14" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="P14" s="6">
+        <v>8.8450622498295039E-5</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>6.8571817211164697E-4</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="U14" s="6">
+        <v>1.3510054044324821E-4</v>
+      </c>
+      <c r="V14" s="6">
+        <v>7.9729353656454911E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E15" s="3">
@@ -1741,7 +1933,7 @@
         <v>144.86430449068999</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J15" s="3">
@@ -1750,17 +1942,34 @@
       <c r="K15" s="3">
         <v>122.7032630945214</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M15" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
+      <c r="O15" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P15" s="6">
+        <v>9.0183213784629648E-5</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>5.4639054870690696E-4</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U15" s="6">
+        <v>1.2781710482353241E-4</v>
+      </c>
+      <c r="V15" s="6">
+        <v>8.6198401991352677E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E16" s="3">
@@ -1770,7 +1979,7 @@
         <v>144.82167579408539</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J16" s="3">
@@ -1779,17 +1988,34 @@
       <c r="K16" s="3">
         <v>108.6723299217339</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M16" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="4"/>
+      <c r="O16" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P16" s="6">
+        <v>9.2219376239589782E-5</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>5.2323089247420529E-4</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="U16" s="6">
+        <v>1.2443272577550871E-4</v>
+      </c>
+      <c r="V16" s="6">
+        <v>9.1678116028961565E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E17" s="3">
@@ -1799,7 +2025,7 @@
         <v>149.10549288061341</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J17" s="3">
@@ -1808,17 +2034,34 @@
       <c r="K17" s="3">
         <v>112.77207706201079</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="5">
         <v>0.99721448467966578</v>
       </c>
-      <c r="M17" s="4">
-        <f t="shared" si="0"/>
-        <v>99.721448467966582</v>
-      </c>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="4"/>
+      <c r="O17" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P17" s="6">
+        <v>8.5356942843666463E-5</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>6.4517021086494511E-4</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U17" s="6">
+        <v>1.213836928698053E-4</v>
+      </c>
+      <c r="V17" s="6">
+        <v>7.4028997501118885E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E18" s="3">
@@ -1828,7 +2071,7 @@
         <v>148.91654983570649</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="J18" s="3">
@@ -1837,17 +2080,34 @@
       <c r="K18" s="3">
         <v>113.98178807947021</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="5">
         <v>1</v>
       </c>
-      <c r="M18" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="4"/>
+      <c r="O18" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P18" s="6">
+        <v>8.742601767126476E-5</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>5.4065447585782613E-4</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="U18" s="6">
+        <v>1.331033592814548E-4</v>
+      </c>
+      <c r="V18" s="6">
+        <v>7.1142868330732127E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E19" s="3">
@@ -1857,7 +2117,7 @@
         <v>137.2727875136911</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J19" s="3">
@@ -1866,17 +2126,34 @@
       <c r="K19" s="3">
         <v>119.08072847682121</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M19" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="4"/>
+      <c r="O19" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P19" s="6">
+        <v>7.6557410587021744E-5</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>8.5767143244083136E-4</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="U19" s="6">
+        <v>1.2588106341208461E-4</v>
+      </c>
+      <c r="V19" s="6">
+        <v>9.6648374952556398E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E20" s="3">
@@ -1886,7 +2163,7 @@
         <v>150.0026286966046</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J20" s="3">
@@ -1895,17 +2172,34 @@
       <c r="K20" s="3">
         <v>120.28684527393141</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="5">
         <v>1</v>
       </c>
-      <c r="M20" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="4"/>
+      <c r="O20" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P20" s="6">
+        <v>8.719879781403104E-5</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>4.4950137736798332E-4</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U20" s="6">
+        <v>1.314733622636012E-4</v>
+      </c>
+      <c r="V20" s="6">
+        <v>6.3127001127431099E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E21" s="3">
@@ -1915,7 +2209,7 @@
         <v>142.2148247535597</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J21" s="3">
@@ -1924,17 +2218,34 @@
       <c r="K21" s="3">
         <v>119.3854786273329</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M21" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="4"/>
+      <c r="O21" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="P21" s="6">
+        <v>9.4192710123153486E-5</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>4.8454346377306909E-4</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="U21" s="6">
+        <v>1.257135650161644E-4</v>
+      </c>
+      <c r="V21" s="6">
+        <v>8.4526032248125754E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E22" s="3">
@@ -1944,7 +2255,7 @@
         <v>137.2438225629792</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J22" s="3">
@@ -1953,17 +2264,34 @@
       <c r="K22" s="3">
         <v>119.4957555689344</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="5">
         <v>1</v>
       </c>
-      <c r="M22" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="4"/>
+      <c r="O22" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="P22" s="6">
+        <v>9.3583604347509375E-5</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>6.8910480660217682E-4</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="U22" s="6">
+        <v>1.2205393305489601E-4</v>
+      </c>
+      <c r="V22" s="6">
+        <v>1.1109788447526961E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="E23" s="3">
@@ -1973,7 +2301,7 @@
         <v>152.57814348302301</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="J23" s="3">
@@ -1982,17 +2310,34 @@
       <c r="K23" s="3">
         <v>114.8200421432872</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="5">
         <v>0.99721448467966578</v>
       </c>
-      <c r="M23" s="4">
-        <f t="shared" si="0"/>
-        <v>99.721448467966582</v>
-      </c>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="4"/>
+      <c r="O23" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="P23" s="6">
+        <v>9.7506568996096778E-5</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>7.2848779667836314E-4</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U23" s="6">
+        <v>1.1028568841265881E-4</v>
+      </c>
+      <c r="V23" s="6">
+        <v>1.1593087544397051E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E24" s="3">
@@ -2002,7 +2347,7 @@
         <v>144.17922234392111</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="J24" s="3">
@@ -2011,17 +2356,34 @@
       <c r="K24" s="3">
         <v>112.41583383503909</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="5">
         <v>1</v>
       </c>
-      <c r="M24" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="4"/>
+      <c r="O24" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="P24" s="6">
+        <v>8.9390024059288832E-5</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>6.5452278075954745E-4</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U24" s="6">
+        <v>1.2272213239451231E-4</v>
+      </c>
+      <c r="V24" s="6">
+        <v>6.4025357704196805E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E25" s="3">
@@ -2031,7 +2393,7 @@
         <v>148.42997261774369</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J25" s="3">
@@ -2040,17 +2402,34 @@
       <c r="K25" s="3">
         <v>125.7609271523179</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M25" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="4"/>
+      <c r="O25" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P25" s="6">
+        <v>9.1455850260113209E-5</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>6.2957446048163518E-4</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U25" s="6">
+        <v>1.3148820591888291E-4</v>
+      </c>
+      <c r="V25" s="6">
+        <v>6.9219512382108289E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E26" s="3">
@@ -2060,7 +2439,7 @@
         <v>146.03740963855421</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J26" s="3">
@@ -2069,17 +2448,34 @@
       <c r="K26" s="3">
         <v>119.7784948826009</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="5">
         <v>0.99581589958158989</v>
       </c>
-      <c r="M26" s="4">
-        <f t="shared" si="0"/>
-        <v>99.581589958158986</v>
-      </c>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="4"/>
+      <c r="O26" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="P26" s="6">
+        <v>8.8310665838610498E-5</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>5.6526107743774161E-4</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="U26" s="6">
+        <v>1.172949587198428E-4</v>
+      </c>
+      <c r="V26" s="6">
+        <v>1.011404424568403E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E27" s="3">
@@ -2089,7 +2485,7 @@
         <v>145.6442661555312</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="J27" s="3">
@@ -2098,17 +2494,34 @@
       <c r="K27" s="3">
         <v>113.5452859723059</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M27" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="4"/>
+      <c r="O27" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="P27" s="6">
+        <v>7.0589975457370908E-5</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>1.2524375115362319E-3</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="U27" s="6">
+        <v>1.2448820086593781E-4</v>
+      </c>
+      <c r="V27" s="6">
+        <v>6.8853616420052764E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E28" s="3">
@@ -2118,7 +2531,7 @@
         <v>145.0289649507119</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="J28" s="3">
@@ -2127,17 +2540,34 @@
       <c r="K28" s="3">
         <v>118.12097531607461</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="5">
         <v>1</v>
       </c>
-      <c r="M28" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="4"/>
+      <c r="O28" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="P28" s="6">
+        <v>8.8722195714730984E-5</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>4.9147664277835162E-4</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="U28" s="6">
+        <v>1.2257170547112881E-4</v>
+      </c>
+      <c r="V28" s="6">
+        <v>8.4712087769224498E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E29" s="3">
@@ -2147,7 +2577,7 @@
         <v>136.14734939759029</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J29" s="3">
@@ -2156,17 +2586,34 @@
       <c r="K29" s="3">
         <v>111.6142022877785</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="5">
         <v>0.99721448467966578</v>
       </c>
-      <c r="M29" s="4">
-        <f t="shared" si="0"/>
-        <v>99.721448467966582</v>
-      </c>
-    </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="4"/>
+      <c r="O29" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="P29" s="6">
+        <v>9.0630142164166891E-5</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>4.832569151022913E-4</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="U29" s="6">
+        <v>1.1912805621076321E-4</v>
+      </c>
+      <c r="V29" s="6">
+        <v>9.2631664213075119E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E30" s="3">
@@ -2176,7 +2623,7 @@
         <v>151.0955969331873</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="J30" s="3">
@@ -2185,17 +2632,34 @@
       <c r="K30" s="3">
         <v>119.20683925346179</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M30" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="31" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="4"/>
+      <c r="O30" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="P30" s="6">
+        <v>8.8798034239177546E-5</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>4.6873180669487091E-4</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U30" s="6">
+        <v>1.2707367681803329E-4</v>
+      </c>
+      <c r="V30" s="6">
+        <v>1.052457409967145E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E31" s="3">
@@ -2205,7 +2669,7 @@
         <v>141.89998904709751</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J31" s="3">
@@ -2214,17 +2678,34 @@
       <c r="K31" s="3">
         <v>112.5925767609874</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="5">
         <v>0.99581589958158989</v>
       </c>
-      <c r="M31" s="4">
-        <f t="shared" si="0"/>
-        <v>99.581589958158986</v>
-      </c>
-    </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="4"/>
+      <c r="O31" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="P31" s="6">
+        <v>8.6785632179424521E-5</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>7.8627690776169896E-4</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="U31" s="6">
+        <v>1.101209863337655E-4</v>
+      </c>
+      <c r="V31" s="6">
+        <v>1.066169818548743E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E32" s="3">
@@ -2234,7 +2715,7 @@
         <v>152.50776560788611</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="J32" s="3">
@@ -2243,17 +2724,34 @@
       <c r="K32" s="3">
         <v>122.1931005418423</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M32" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M32" s="4"/>
+      <c r="O32" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P32" s="6">
+        <v>7.3018896158951989E-5</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>1.041446905582501E-3</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="U32" s="6">
+        <v>1.1631411971062931E-4</v>
+      </c>
+      <c r="V32" s="6">
+        <v>8.2252014019582834E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E33" s="3">
@@ -2263,7 +2761,7 @@
         <v>141.51168674698789</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="J33" s="3">
@@ -2272,17 +2770,34 @@
       <c r="K33" s="3">
         <v>124.2636845273931</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="5">
         <v>0.99581589958158989</v>
       </c>
-      <c r="M33" s="4">
-        <f t="shared" si="0"/>
-        <v>99.581589958158986</v>
-      </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="4"/>
+      <c r="O33" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="P33" s="6">
+        <v>9.7832841476558539E-5</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>6.4295127821008898E-4</v>
+      </c>
+      <c r="T33" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="U33" s="6">
+        <v>1.1691816707344799E-4</v>
+      </c>
+      <c r="V33" s="6">
+        <v>8.4187107257652205E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E34" s="3">
@@ -2292,7 +2807,7 @@
         <v>141.1243318729463</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="J34" s="3">
@@ -2301,17 +2816,34 @@
       <c r="K34" s="3">
         <v>122.28586393738711</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M34" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="4"/>
+      <c r="O34" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="P34" s="6">
+        <v>8.6104732237515035E-5</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>5.4376201213406517E-4</v>
+      </c>
+      <c r="T34" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="U34" s="6">
+        <v>1.186602763214805E-4</v>
+      </c>
+      <c r="V34" s="6">
+        <v>8.439045204805169E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E35" s="3">
@@ -2321,7 +2853,7 @@
         <v>141.574282584885</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="J35" s="3">
@@ -2330,17 +2862,34 @@
       <c r="K35" s="3">
         <v>120.4993076459964</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M35" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="4"/>
+      <c r="O35" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="P35" s="6">
+        <v>9.4946517116823912E-5</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>4.8675777407309213E-4</v>
+      </c>
+      <c r="T35" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U35" s="6">
+        <v>1.1581103370376969E-4</v>
+      </c>
+      <c r="V35" s="6">
+        <v>9.014769022625003E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E36" s="3">
@@ -2350,7 +2899,7 @@
         <v>146.70938116100771</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="J36" s="3">
@@ -2359,17 +2908,34 @@
       <c r="K36" s="3">
         <v>113.2963455749548</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="5">
         <v>0.99860917941585536</v>
       </c>
-      <c r="M36" s="4">
-        <f t="shared" si="0"/>
-        <v>99.860917941585541</v>
-      </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M36" s="4"/>
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="P36" s="6">
+        <v>1.049073753290893E-4</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>5.1216718158469629E-4</v>
+      </c>
+      <c r="T36" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="U36" s="6">
+        <v>1.165808712408225E-4</v>
+      </c>
+      <c r="V36" s="6">
+        <v>1.025380525361276E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E37" s="3">
@@ -2379,7 +2945,7 @@
         <v>142.65382803943041</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="J37" s="3">
@@ -2388,17 +2954,34 @@
       <c r="K37" s="3">
         <v>120.343925346177</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M37" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M37" s="4"/>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="P37" s="6">
+        <v>9.4872410336933956E-5</v>
+      </c>
+      <c r="Q37" s="6">
+        <v>6.3429878120420293E-4</v>
+      </c>
+      <c r="T37" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="U37" s="6">
+        <v>1.149138524556614E-4</v>
+      </c>
+      <c r="V37" s="6">
+        <v>1.093108640349606E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E38" s="3">
@@ -2408,7 +2991,7 @@
         <v>146.14921686746979</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="J38" s="3">
@@ -2417,17 +3000,34 @@
       <c r="K38" s="3">
         <v>118.42411800120411</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M38" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M38" s="4"/>
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="P38" s="6">
+        <v>8.7780759900966401E-5</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>7.3159061510171225E-4</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="U38" s="6">
+        <v>1.161721732644664E-4</v>
+      </c>
+      <c r="V38" s="6">
+        <v>9.0313277977909076E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E39" s="3">
@@ -2437,7 +3037,7 @@
         <v>149.293587075575</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="J39" s="3">
@@ -2446,17 +3046,34 @@
       <c r="K39" s="3">
         <v>127.0351776038531</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="5">
         <v>0.99439775910364148</v>
       </c>
-      <c r="M39" s="4">
-        <f t="shared" si="0"/>
-        <v>99.439775910364148</v>
-      </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M39" s="4"/>
+      <c r="O39" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P39" s="6">
+        <v>8.9922618268825606E-5</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>5.4042864346485326E-4</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="U39" s="6">
+        <v>1.2013804201188541E-4</v>
+      </c>
+      <c r="V39" s="6">
+        <v>1.1092219520759631E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E40" s="3">
@@ -2466,7 +3083,7 @@
         <v>143.4984501642935</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="J40" s="3">
@@ -2475,17 +3092,34 @@
       <c r="K40" s="3">
         <v>117.07953642384101</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="5">
         <v>0.99583911234396671</v>
       </c>
-      <c r="M40" s="4">
-        <f t="shared" si="0"/>
-        <v>99.583911234396666</v>
-      </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="4"/>
+      <c r="O40" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="P40" s="6">
+        <v>9.0462234735740505E-5</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>3.9353551819460011E-4</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="U40" s="6">
+        <v>1.093439754658021E-4</v>
+      </c>
+      <c r="V40" s="6">
+        <v>1.2470696650656221E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E41" s="3">
@@ -2495,7 +3129,7 @@
         <v>149.89188389923331</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="J41" s="3">
@@ -2504,17 +3138,34 @@
       <c r="K41" s="3">
         <v>121.0951113786876</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M41" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="4"/>
+      <c r="O41" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="P41" s="6">
+        <v>8.9831755682805476E-5</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>4.8466311030854992E-4</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="U41" s="6">
+        <v>1.3200713218473401E-4</v>
+      </c>
+      <c r="V41" s="6">
+        <v>6.0641842384086134E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="E42" s="3">
@@ -2524,7 +3175,7 @@
         <v>140.73727272727271</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="J42" s="3">
@@ -2533,17 +3184,34 @@
       <c r="K42" s="3">
         <v>116.6958759783263</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="5">
         <v>0.99580419580419577</v>
       </c>
-      <c r="M42" s="4">
-        <f t="shared" si="0"/>
-        <v>99.580419580419573</v>
-      </c>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="4"/>
+      <c r="O42" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P42" s="6">
+        <v>9.2695216664067024E-5</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>6.0301770627685174E-4</v>
+      </c>
+      <c r="T42" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="U42" s="6">
+        <v>1.243893078757672E-4</v>
+      </c>
+      <c r="V42" s="6">
+        <v>6.4137284660238365E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="E43" s="3">
@@ -2553,7 +3221,7 @@
         <v>146.27437568455639</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="J43" s="3">
@@ -2562,17 +3230,34 @@
       <c r="K43" s="3">
         <v>116.5089825406382</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M43" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="4"/>
+      <c r="O43" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="P43" s="6">
+        <v>9.2772346724412987E-5</v>
+      </c>
+      <c r="Q43" s="6">
+        <v>5.581988107419563E-4</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="U43" s="6">
+        <v>1.2796915013832901E-4</v>
+      </c>
+      <c r="V43" s="6">
+        <v>7.842184876207509E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="E44" s="3">
@@ -2582,7 +3267,7 @@
         <v>150.5310952902519</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="J44" s="3">
@@ -2591,17 +3276,34 @@
       <c r="K44" s="3">
         <v>119.2434617700181</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M44" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="4"/>
+      <c r="O44" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="P44" s="6">
+        <v>8.2377915262745369E-5</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>6.9406158225527518E-4</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="U44" s="6">
+        <v>1.26623201515188E-4</v>
+      </c>
+      <c r="V44" s="6">
+        <v>8.4674089676561458E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E45" s="3">
@@ -2611,7 +3313,7 @@
         <v>143.680443592552</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J45" s="3">
@@ -2620,17 +3322,34 @@
       <c r="K45" s="3">
         <v>118.1418121613486</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="5">
         <v>0.99721448467966578</v>
       </c>
-      <c r="M45" s="4">
-        <f t="shared" si="0"/>
-        <v>99.721448467966582</v>
-      </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M45" s="4"/>
+      <c r="O45" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="P45" s="6">
+        <v>7.7895032348555582E-5</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>8.5500559766936283E-4</v>
+      </c>
+      <c r="T45" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U45" s="6">
+        <v>1.14893492568111E-4</v>
+      </c>
+      <c r="V45" s="6">
+        <v>1.1309888794191561E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E46" s="3">
@@ -2640,7 +3359,7 @@
         <v>150.5702683461117</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="J46" s="3">
@@ -2649,17 +3368,34 @@
       <c r="K46" s="3">
         <v>122.2600361228176</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="5">
         <v>0.99721448467966578</v>
       </c>
-      <c r="M46" s="4">
-        <f t="shared" si="0"/>
-        <v>99.721448467966582</v>
-      </c>
-    </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M46" s="4"/>
+      <c r="O46" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="P46" s="6">
+        <v>9.4696631574829493E-5</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>4.8516569375974141E-4</v>
+      </c>
+      <c r="T46" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="U46" s="6">
+        <v>1.2503425381630269E-4</v>
+      </c>
+      <c r="V46" s="6">
+        <v>8.1257762125139742E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E47" s="3">
@@ -2669,7 +3405,7 @@
         <v>139.9791018619934</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="J47" s="3">
@@ -2678,17 +3414,34 @@
       <c r="K47" s="3">
         <v>123.88800722456349</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47" s="5">
         <v>0.9972067039106145</v>
       </c>
-      <c r="M47" s="4">
-        <f t="shared" si="0"/>
-        <v>99.720670391061446</v>
-      </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="4"/>
+      <c r="O47" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="P47" s="6">
+        <v>8.7790596264620413E-5</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>8.4764028747091945E-4</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="U47" s="6">
+        <v>1.0294523615547651E-4</v>
+      </c>
+      <c r="V47" s="6">
+        <v>1.46714595666021E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="E48" s="3">
@@ -2698,7 +3451,7 @@
         <v>144.6483625410734</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="J48" s="3">
@@ -2707,17 +3460,34 @@
       <c r="K48" s="3">
         <v>112.4657074051776</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="5">
         <v>1</v>
       </c>
-      <c r="M48" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="4"/>
+      <c r="O48" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="P48" s="6">
+        <v>7.541054372573891E-5</v>
+      </c>
+      <c r="Q48" s="6">
+        <v>1.0276441621686679E-3</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="U48" s="6">
+        <v>1.168407577686567E-4</v>
+      </c>
+      <c r="V48" s="6">
+        <v>8.7897910071153417E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="E49" s="3">
@@ -2727,7 +3497,7 @@
         <v>149.1498138006572</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="J49" s="3">
@@ -2736,17 +3506,34 @@
       <c r="K49" s="3">
         <v>112.1260686333534</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="5">
         <v>0.99860917941585536</v>
       </c>
-      <c r="M49" s="4">
-        <f t="shared" si="0"/>
-        <v>99.860917941585541</v>
-      </c>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M49" s="4"/>
+      <c r="O49" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P49" s="6">
+        <v>8.6614102641646181E-5</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>6.6858373015753507E-4</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="U49" s="6">
+        <v>1.221622187447097E-4</v>
+      </c>
+      <c r="V49" s="6">
+        <v>9.8622951537373168E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E50" s="3">
@@ -2756,7 +3543,7 @@
         <v>154.67331872946329</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="J50" s="3">
@@ -2765,17 +3552,34 @@
       <c r="K50" s="3">
         <v>117.76434075857919</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M50" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="4"/>
+      <c r="O50" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P50" s="6">
+        <v>9.1993100829013512E-5</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>4.7410528106787508E-4</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="U50" s="6">
+        <v>1.187631280360972E-4</v>
+      </c>
+      <c r="V50" s="6">
+        <v>1.057709492025047E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="E51" s="3">
@@ -2785,7 +3589,7 @@
         <v>146.68242059145669</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="J51" s="3">
@@ -2794,17 +3598,34 @@
       <c r="K51" s="3">
         <v>125.05628537025891</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51" s="5">
         <v>0.99298737727910236</v>
       </c>
-      <c r="M51" s="4">
-        <f t="shared" si="0"/>
-        <v>99.298737727910236</v>
-      </c>
-    </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M51" s="4"/>
+      <c r="O51" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="P51" s="6">
+        <v>9.8045923640924297E-5</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>6.8065822022607349E-4</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="U51" s="6">
+        <v>1.312275112482064E-4</v>
+      </c>
+      <c r="V51" s="6">
+        <v>8.4211498440781734E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="E52" s="3">
@@ -2814,7 +3635,7 @@
         <v>130.6130887185104</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="J52" s="3">
@@ -2823,17 +3644,34 @@
       <c r="K52" s="3">
         <v>115.4081216134859</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="5">
         <v>1</v>
       </c>
-      <c r="M52" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="4"/>
+      <c r="O52" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="P52" s="6">
+        <v>8.7830486481270772E-5</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>5.0366963897650755E-4</v>
+      </c>
+      <c r="T52" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="U52" s="6">
+        <v>1.2471372369474211E-4</v>
+      </c>
+      <c r="V52" s="6">
+        <v>7.4555923734151745E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="E53" s="3">
@@ -2843,7 +3681,7 @@
         <v>143.91588170865279</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="J53" s="3">
@@ -2852,17 +3690,34 @@
       <c r="K53" s="3">
         <v>110.6394220349187</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53" s="5">
         <v>0.99860917941585536</v>
       </c>
-      <c r="M53" s="4">
-        <f t="shared" si="0"/>
-        <v>99.860917941585541</v>
-      </c>
-    </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M53" s="4"/>
+      <c r="O53" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="P53" s="6">
+        <v>8.4895616735961013E-5</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>7.6926540067693997E-4</v>
+      </c>
+      <c r="T53" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="U53" s="6">
+        <v>1.113379617603689E-4</v>
+      </c>
+      <c r="V53" s="6">
+        <v>9.5659094739302373E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E54" s="3">
@@ -2872,7 +3727,7 @@
         <v>142.34866922234389</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="J54" s="3">
@@ -2881,17 +3736,34 @@
       <c r="K54" s="3">
         <v>122.0827513546057</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L54" s="5">
         <v>0.99580419580419577</v>
       </c>
-      <c r="M54" s="4">
-        <f t="shared" si="0"/>
-        <v>99.580419580419573</v>
-      </c>
-    </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M54" s="4"/>
+      <c r="O54" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="P54" s="6">
+        <v>8.2473087820237107E-5</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>7.836208816430916E-4</v>
+      </c>
+      <c r="T54" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="U54" s="6">
+        <v>1.167654447349066E-4</v>
+      </c>
+      <c r="V54" s="6">
+        <v>9.5188505308882313E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="E55" s="3">
@@ -2901,7 +3773,7 @@
         <v>144.2873384446878</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="J55" s="3">
@@ -2910,15 +3782,32 @@
       <c r="K55" s="3">
         <v>121.8412703190849</v>
       </c>
-      <c r="L55" s="4">
+      <c r="L55" s="5">
         <v>0.99860529986053004</v>
       </c>
-      <c r="M55" s="4">
-        <f t="shared" si="0"/>
-        <v>99.86052998605301</v>
-      </c>
-    </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M55" s="4"/>
+      <c r="O55" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="P55" s="6">
+        <v>9.5896646998853356E-5</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>5.9735956864187512E-4</v>
+      </c>
+      <c r="T55" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U55" s="6">
+        <v>1.279191349390201E-4</v>
+      </c>
+      <c r="V55" s="6">
+        <v>8.439628751452543E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2945,12 +3834,31 @@
         <f>AVERAGE(L6:L55)</f>
         <v>0.99748679962917774</v>
       </c>
-      <c r="M57" s="3">
-        <f>AVERAGE(M6:M55)</f>
-        <v>99.748679962917763</v>
-      </c>
-    </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M57" s="3"/>
+      <c r="O57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P57" s="6">
+        <f>AVERAGE(P6:P55)</f>
+        <v>8.8834506767543616E-5</v>
+      </c>
+      <c r="Q57" s="6">
+        <f>AVERAGE(Q6:Q55)</f>
+        <v>6.3209977823717772E-4</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U57" s="6">
+        <f>AVERAGE(U6:U55)</f>
+        <v>1.2191839352985973E-4</v>
+      </c>
+      <c r="V57" s="6">
+        <f>AVERAGE(V6:V55)</f>
+        <v>8.8895756218133957E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2977,12 +3885,31 @@
         <f>_xlfn.STDEV.S(L6:L55)</f>
         <v>1.7424191707030769E-3</v>
       </c>
-      <c r="M58" s="3">
-        <f>_xlfn.STDEV.S(M6:M55)</f>
-        <v>0.17424191707030973</v>
-      </c>
-    </row>
-    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M58" s="3"/>
+      <c r="O58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P58" s="6">
+        <f>_xlfn.STDEV.S(P6:P55)</f>
+        <v>6.4828512941912346E-6</v>
+      </c>
+      <c r="Q58" s="6">
+        <f>_xlfn.STDEV.S(Q6:Q55)</f>
+        <v>1.7187858033729611E-4</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U58" s="6">
+        <f>_xlfn.STDEV.S(U6:U55)</f>
+        <v>7.1459789974840207E-6</v>
+      </c>
+      <c r="V58" s="6">
+        <f>_xlfn.STDEV.S(V6:V55)</f>
+        <v>1.8171701498687141E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="4:22" x14ac:dyDescent="0.25">
       <c r="I62" s="4" t="s">
         <v>8</v>
       </c>
@@ -2990,7 +3917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:22" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
         <v>6</v>
       </c>
@@ -3003,7 +3930,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:22" x14ac:dyDescent="0.25">
       <c r="H64" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
features significance for small cities & mun
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-5.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-5.xlsx
@@ -1444,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W63" sqref="W63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,7 +3830,7 @@
         <f>AVERAGE(K6:K55)</f>
         <v>117.60700541842267</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57" s="5">
         <f>AVERAGE(L6:L55)</f>
         <v>0.99748679962917774</v>
       </c>
@@ -3881,7 +3881,7 @@
         <f>_xlfn.STDEV.S(K6:K55)</f>
         <v>4.506765948772407</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58" s="5">
         <f>_xlfn.STDEV.S(L6:L55)</f>
         <v>1.7424191707030769E-3</v>
       </c>

</xml_diff>